<commit_message>
Mejora Matriz de Riesgo
</commit_message>
<xml_diff>
--- a/trabajos.inacap.2019/Preparacion y evaluacion de proyecto (PEP)/Acumulado/Matriz de Riesgo.xlsx
+++ b/trabajos.inacap.2019/Preparacion y evaluacion de proyecto (PEP)/Acumulado/Matriz de Riesgo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mis Cosas\Estudios\Universidad\Semestre 3\Sistema de Informacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D443E53A-8429-4ECF-942D-B783229EE1A6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F6399B-3588-4F7D-8471-B23EEFCF69F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="285" windowWidth="20490" windowHeight="10635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
   <si>
     <t>Procesos</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Permanente(Pe)</t>
+  </si>
+  <si>
+    <t>Objetivos Especificos</t>
   </si>
 </sst>
 </file>
@@ -207,7 +210,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -230,22 +233,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,154 +643,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AC31"/>
+  <dimension ref="A2:AE31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2" t="s">
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="3"/>
+      <c r="O3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="R3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="3"/>
+      <c r="T3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2" t="s">
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="X3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="W3" s="2"/>
-      <c r="X3" s="3" t="s">
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="2" t="s">
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2" t="s">
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AC3" s="2"/>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="AE3" s="3"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="1" t="s">
+      <c r="M4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U4" s="2"/>
-      <c r="V4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="W4" s="3"/>
       <c r="X4" s="1" t="s">
         <v>17</v>
       </c>
@@ -726,78 +811,84 @@
       <c r="AC4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="AD4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -856,7 +947,7 @@
       <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="2">
         <v>1</v>
       </c>
       <c r="C27" t="s">
@@ -908,29 +999,30 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="M3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="G2:O2"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="V2:AC2"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="P2:U2"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="P3:Q4"/>
-    <mergeCell ref="E2:F4"/>
-    <mergeCell ref="G3:H4"/>
-    <mergeCell ref="A5:B8"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
+  <mergeCells count="23">
     <mergeCell ref="A9:B12"/>
     <mergeCell ref="A13:B16"/>
     <mergeCell ref="A17:B20"/>
     <mergeCell ref="A2:B4"/>
     <mergeCell ref="C2:D4"/>
+    <mergeCell ref="I3:J4"/>
+    <mergeCell ref="A5:B8"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="E2:F4"/>
+    <mergeCell ref="G2:H4"/>
+    <mergeCell ref="O3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="I2:Q2"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="X2:AE2"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="R2:W2"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="R3:S4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se modifica la matriz de riesgo de PEP
</commit_message>
<xml_diff>
--- a/trabajos.inacap.2019/Preparacion y evaluacion de proyecto (PEP)/Acumulado/Matriz de Riesgo.xlsx
+++ b/trabajos.inacap.2019/Preparacion y evaluacion de proyecto (PEP)/Acumulado/Matriz de Riesgo.xlsx
@@ -8,25 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\GitHub INACAP\inacap.2019\trabajos.inacap.2019\Preparacion y evaluacion de proyecto (PEP)\Acumulado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088D30C3-936B-467B-AA1A-33B8BE058AD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6978E6A4-DA95-4099-B06B-6AB3ED75D389}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz de riesgo" sheetId="1" r:id="rId1"/>
     <sheet name="Escalas y Antecendes de Mencion" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
   <si>
     <t>Procesos</t>
   </si>
@@ -46,9 +51,6 @@
     <t>Impacto</t>
   </si>
   <si>
-    <t>Severidad del Riesgo</t>
-  </si>
-  <si>
     <t>Valor</t>
   </si>
   <si>
@@ -95,6 +97,158 @@
   </si>
   <si>
     <t>Clasific.</t>
+  </si>
+  <si>
+    <t>Cambios Contaste del 
+Grupo de Trabajo.</t>
+  </si>
+  <si>
+    <t>Falla de Comunicación con 
+la Empresa.</t>
+  </si>
+  <si>
+    <t>Problema al Implementar en 
+Recusos de la Empresa.</t>
+  </si>
+  <si>
+    <t>Programacion</t>
+  </si>
+  <si>
+    <t>Implementacion</t>
+  </si>
+  <si>
+    <t>Ejecucion</t>
+  </si>
+  <si>
+    <t>Documentacion</t>
+  </si>
+  <si>
+    <t>Tomar requerimiento de las pruebas con la empresa.</t>
+  </si>
+  <si>
+    <t>Proponer la fecha limite para 
+culminar este proyecto.</t>
+  </si>
+  <si>
+    <t>Mantiener el orden cronologico 
+de las actividades.</t>
+  </si>
+  <si>
+    <t>Implementacion de 
+Software</t>
+  </si>
+  <si>
+    <t>Cronogramas Programado</t>
+  </si>
+  <si>
+    <t>Iteraciones.</t>
+  </si>
+  <si>
+    <t>Programacion de Tiempo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Control </t>
+  </si>
+  <si>
+    <t>Manipulacion erronea en el Cronograma.</t>
+  </si>
+  <si>
+    <t>Manipulacion de Fecha del Termino del Proyecto Continua.</t>
+  </si>
+  <si>
+    <t>Gestionar y prueba distintas 
+etapas tempranas del software.</t>
+  </si>
+  <si>
+    <t>Falla Numerosas pruebas del 
+Software.</t>
+  </si>
+  <si>
+    <t>Cliente no Propone Informacion para un feed-back.</t>
+  </si>
+  <si>
+    <t>Organización del Grupo de proyecto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registo de existencia </t>
+  </si>
+  <si>
+    <t>Conservacion de 
+Documentacion</t>
+  </si>
+  <si>
+    <t>Entrevistas</t>
+  </si>
+  <si>
+    <t>Etapas Tardia de Iteraciones.</t>
+  </si>
+  <si>
+    <t>Etapas Temprana de Iteraciones.</t>
+  </si>
+  <si>
+    <t>Asistencia</t>
+  </si>
+  <si>
+    <t>Atrasos continuos de la
+Documentacion.</t>
+  </si>
+  <si>
+    <t>Empresa sin Vision Fija del 
+Proyecto.</t>
+  </si>
+  <si>
+    <t>Marcha Blanca sin
+Tiempo Estimado.</t>
+  </si>
+  <si>
+    <t>Inserción del Software</t>
+  </si>
+  <si>
+    <t>Severidad 
+del Riesgo</t>
+  </si>
+  <si>
+    <t>Gestiona los documentos del proyecto y la Informacion de la Empresa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comprueba a las persona 
+mantiene sus rubros asignados. </t>
+  </si>
+  <si>
+    <t>Mantiener comunicación 
+con la empresa.</t>
+  </si>
+  <si>
+    <t>Busca nuevas expectativas 
+con el proyecto.</t>
+  </si>
+  <si>
+    <t>Implementar el software 
+en los recursos especificos.</t>
+  </si>
+  <si>
+    <t>Probable</t>
+  </si>
+  <si>
+    <t>Moderad.</t>
+  </si>
+  <si>
+    <t>Improb.</t>
+  </si>
+  <si>
+    <t>Mayores</t>
+  </si>
+  <si>
+    <t>Menores</t>
+  </si>
+  <si>
+    <t>Alto</t>
+  </si>
+  <si>
+    <t>Moderado</t>
+  </si>
+  <si>
+    <t>Extremo</t>
   </si>
 </sst>
 </file>
@@ -117,7 +271,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +296,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -280,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -289,62 +455,98 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -940,13 +1142,19 @@
   </sheetPr>
   <dimension ref="A2:AF27"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B8"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21:T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" customWidth="1"/>
+    <col min="15" max="15" width="8" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" customWidth="1"/>
     <col min="20" max="20" width="7.7109375" customWidth="1"/>
     <col min="21" max="21" width="8.42578125" customWidth="1"/>
     <col min="22" max="22" width="8.140625" customWidth="1"/>
@@ -954,289 +1162,970 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="19" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="15"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="23"/>
+      <c r="I3" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="17"/>
+      <c r="O3" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="20" t="s">
+      <c r="S3" s="9"/>
+      <c r="T3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="X3" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2" s="22"/>
-      <c r="AF2" s="22"/>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="5" t="s">
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF3" s="9"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="14" t="s">
+      <c r="L4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" s="9">
+        <v>4</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="N5" s="9">
         <v>3</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14" t="s">
+      <c r="O5" s="29">
+        <f>L5*N5</f>
+        <v>12</v>
+      </c>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="R5" s="32"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" s="9">
+        <v>3</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="9">
+        <v>3</v>
+      </c>
+      <c r="O7" s="29">
+        <f t="shared" ref="O7" si="0">L7*N7</f>
+        <v>9</v>
+      </c>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="R7" s="33"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="33"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="34"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+    </row>
+    <row r="9" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="L9" s="9">
         <v>4</v>
       </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14" t="s">
+      <c r="M9" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="N9" s="9">
+        <v>2</v>
+      </c>
+      <c r="O9" s="29">
+        <f t="shared" ref="O9" si="1">L9*N9</f>
+        <v>8</v>
+      </c>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="R9" s="33"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="34"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="33"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="34"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L11" s="9">
+        <v>3</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="N11" s="9">
+        <v>3</v>
+      </c>
+      <c r="O11" s="29">
+        <f t="shared" ref="O11" si="2">L11*N11</f>
+        <v>9</v>
+      </c>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="R11" s="33"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="34"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="33"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="34"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+    </row>
+    <row r="13" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="L13" s="9">
+        <v>4</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="N13" s="9">
+        <v>3</v>
+      </c>
+      <c r="O13" s="29">
+        <f t="shared" ref="O13" si="3">L13*N13</f>
+        <v>12</v>
+      </c>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="R13" s="33"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="34"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+    </row>
+    <row r="14" spans="1:32" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="33"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="34"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="L15" s="9">
+        <v>2</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="N15" s="9">
+        <v>3</v>
+      </c>
+      <c r="O15" s="30">
+        <f t="shared" ref="O15" si="4">L15*N15</f>
         <v>6</v>
       </c>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="X3" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB3" s="11"/>
-      <c r="AC3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF3" s="4"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="1" t="s">
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="R15" s="33"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="34"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="33"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="34"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="L17" s="9">
+        <v>2</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="N17" s="9">
+        <v>3</v>
+      </c>
+      <c r="O17" s="30">
+        <f t="shared" ref="O17" si="5">L17*N17</f>
+        <v>6</v>
+      </c>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="R17" s="33"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="34"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="34"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="L19" s="9">
+        <v>4</v>
+      </c>
+      <c r="M19" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="N19" s="9">
+        <v>2</v>
+      </c>
+      <c r="O19" s="29">
+        <f t="shared" ref="O19" si="6">L19*N19</f>
+        <v>8</v>
+      </c>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="R19" s="33"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="34"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="33"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="34"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="L21" s="9">
+        <v>4</v>
+      </c>
+      <c r="M21" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="N21" s="9">
+        <v>4</v>
+      </c>
+      <c r="O21" s="31">
+        <f t="shared" ref="O21" si="7">L21*N21</f>
         <v>16</v>
       </c>
-      <c r="Z4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA4" s="1" t="s">
+      <c r="P21" s="31"/>
+      <c r="Q21" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="R21" s="33"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="34"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="33"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="34"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="9"/>
+      <c r="G23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="9"/>
+      <c r="I23" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="L23" s="9">
+        <v>4</v>
+      </c>
+      <c r="M23" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="N23" s="9">
+        <v>4</v>
+      </c>
+      <c r="O23" s="31">
+        <f t="shared" ref="O23" si="8">L23*N23</f>
         <v>16</v>
       </c>
-      <c r="AB4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="P23" s="31"/>
+      <c r="Q23" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="R23" s="33"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="34"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="4"/>
+      <c r="X23" s="4"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="33"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="34"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="4"/>
+      <c r="W24" s="4"/>
+      <c r="X24" s="4"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="G2:Q2"/>
-    <mergeCell ref="G3:H4"/>
-    <mergeCell ref="C5:D8"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="E7:F8"/>
-    <mergeCell ref="G5:H6"/>
-    <mergeCell ref="O3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
+  <mergeCells count="178">
+    <mergeCell ref="W21:W22"/>
+    <mergeCell ref="W23:W24"/>
+    <mergeCell ref="X5:X6"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="X15:X16"/>
+    <mergeCell ref="X17:X18"/>
+    <mergeCell ref="X19:X20"/>
+    <mergeCell ref="X21:X22"/>
+    <mergeCell ref="X23:X24"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="W7:W8"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="W11:W12"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="W15:W16"/>
+    <mergeCell ref="W17:W18"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="U23:U24"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="V11:V12"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="V15:V16"/>
+    <mergeCell ref="V17:V18"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="V21:V22"/>
+    <mergeCell ref="V23:V24"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="U15:U16"/>
+    <mergeCell ref="U17:U18"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="U21:U22"/>
+    <mergeCell ref="R23:S24"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="T17:T18"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="T21:T22"/>
+    <mergeCell ref="T23:T24"/>
+    <mergeCell ref="R5:S6"/>
+    <mergeCell ref="R7:S8"/>
+    <mergeCell ref="R9:S10"/>
+    <mergeCell ref="R11:S12"/>
+    <mergeCell ref="R13:S14"/>
+    <mergeCell ref="R15:S16"/>
+    <mergeCell ref="R17:S18"/>
+    <mergeCell ref="R19:S20"/>
+    <mergeCell ref="R21:S22"/>
+    <mergeCell ref="A2:B4"/>
+    <mergeCell ref="C2:D4"/>
     <mergeCell ref="AE3:AF3"/>
     <mergeCell ref="Y2:AF2"/>
     <mergeCell ref="T3:V3"/>
@@ -1247,16 +2136,112 @@
     <mergeCell ref="AC3:AD3"/>
     <mergeCell ref="R3:S4"/>
     <mergeCell ref="W3:W4"/>
+    <mergeCell ref="G2:Q2"/>
+    <mergeCell ref="G3:H4"/>
+    <mergeCell ref="O3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="I3:J4"/>
-    <mergeCell ref="A5:B8"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="E2:F4"/>
-    <mergeCell ref="A9:B12"/>
-    <mergeCell ref="A13:B16"/>
+    <mergeCell ref="E17:F18"/>
+    <mergeCell ref="E19:F20"/>
+    <mergeCell ref="A21:B24"/>
+    <mergeCell ref="I5:J6"/>
+    <mergeCell ref="A5:B16"/>
+    <mergeCell ref="I13:J14"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="I17:J18"/>
+    <mergeCell ref="I19:J20"/>
     <mergeCell ref="A17:B20"/>
-    <mergeCell ref="A2:B4"/>
-    <mergeCell ref="C2:D4"/>
+    <mergeCell ref="C5:D8"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="E7:F8"/>
+    <mergeCell ref="G5:H6"/>
+    <mergeCell ref="I21:J22"/>
+    <mergeCell ref="I23:J24"/>
+    <mergeCell ref="C9:D12"/>
+    <mergeCell ref="C13:D16"/>
+    <mergeCell ref="C17:D20"/>
+    <mergeCell ref="C21:D24"/>
+    <mergeCell ref="I7:J8"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="I11:J12"/>
+    <mergeCell ref="G15:H16"/>
+    <mergeCell ref="G17:H18"/>
+    <mergeCell ref="G19:H20"/>
+    <mergeCell ref="G21:H22"/>
+    <mergeCell ref="G23:H24"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="G9:H10"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="E13:F14"/>
+    <mergeCell ref="E21:F22"/>
+    <mergeCell ref="E23:F24"/>
+    <mergeCell ref="E9:F10"/>
+    <mergeCell ref="E11:F12"/>
+    <mergeCell ref="E15:F16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="O5:P6"/>
+    <mergeCell ref="O7:P8"/>
+    <mergeCell ref="O9:P10"/>
+    <mergeCell ref="O11:P12"/>
+    <mergeCell ref="O13:P14"/>
+    <mergeCell ref="O15:P16"/>
+    <mergeCell ref="O17:P18"/>
+    <mergeCell ref="O19:P20"/>
+    <mergeCell ref="O21:P22"/>
+    <mergeCell ref="O23:P24"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="Q17:Q18"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="Q21:Q22"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="Q13:Q14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1269,7 +2254,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="M16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se actualiza la Matriz de Riesgo
</commit_message>
<xml_diff>
--- a/trabajos.inacap.2019/Preparacion y evaluacion de proyecto (PEP)/Acumulado/Matriz de Riesgo.xlsx
+++ b/trabajos.inacap.2019/Preparacion y evaluacion de proyecto (PEP)/Acumulado/Matriz de Riesgo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\GitHub INACAP\inacap.2019\trabajos.inacap.2019\Preparacion y evaluacion de proyecto (PEP)\Acumulado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6978E6A4-DA95-4099-B06B-6AB3ED75D389}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E42AE4-25F1-4521-993E-4100D65DE316}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="90">
   <si>
     <t>Procesos</t>
   </si>
@@ -249,6 +249,83 @@
   </si>
   <si>
     <t>Extremo</t>
+  </si>
+  <si>
+    <t>El Grupo de Proyecto fija 
+el termino del proyecto.</t>
+  </si>
+  <si>
+    <t>El Grupo de Proyecto se planifica actividades futuras.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tanto la Empresa y el Grupo de 
+Proyecto crean una retroalimentacion. </t>
+  </si>
+  <si>
+    <t>Se archivan todos los documentos 
+de ingresos de datos existentes.</t>
+  </si>
+  <si>
+    <t>Se Busca mejorar el personal 
+para la mejora del proyecto.</t>
+  </si>
+  <si>
+    <t>El Programador realiza pruebas de Software.</t>
+  </si>
+  <si>
+    <t>Una persona del grupo interviene en 
+buscar una comunicación mas efectiva.</t>
+  </si>
+  <si>
+    <t>Una persona del grupo intenta mostar 
+y guiar hacia la mejor vision.</t>
+  </si>
+  <si>
+    <t>Existe un encargado que 
+posee registro de recursos.</t>
+  </si>
+  <si>
+    <t>El Cronograma indica tiempo 
+para efectuar esta tarea.</t>
+  </si>
+  <si>
+    <t>Pd</t>
+  </si>
+  <si>
+    <t>Pe</t>
+  </si>
+  <si>
+    <t>Oc</t>
+  </si>
+  <si>
+    <t>Cr</t>
+  </si>
+  <si>
+    <t>Dt</t>
+  </si>
+  <si>
+    <t>Pv</t>
+  </si>
+  <si>
+    <t>Sa</t>
+  </si>
+  <si>
+    <t>At</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>Optimo</t>
+  </si>
+  <si>
+    <t>Mas Que Regular</t>
+  </si>
+  <si>
+    <t>Bueno</t>
+  </si>
+  <si>
+    <t>Regular</t>
   </si>
 </sst>
 </file>
@@ -271,7 +348,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,18 +375,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -442,11 +537,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -455,30 +563,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -488,65 +647,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1142,8 +1274,8 @@
   </sheetPr>
   <dimension ref="A2:AF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21:T22"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AB23" sqref="AB23:AB24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,10 +1287,12 @@
     <col min="14" max="14" width="8.42578125" customWidth="1"/>
     <col min="15" max="15" width="8" customWidth="1"/>
     <col min="16" max="16" width="6.140625" customWidth="1"/>
+    <col min="19" max="19" width="23.42578125" customWidth="1"/>
     <col min="20" max="20" width="7.7109375" customWidth="1"/>
     <col min="21" max="21" width="8.42578125" customWidth="1"/>
     <col min="22" max="22" width="8.140625" customWidth="1"/>
     <col min="23" max="23" width="6.7109375" customWidth="1"/>
+    <col min="24" max="24" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -1170,71 +1304,71 @@
         <v>1</v>
       </c>
       <c r="D2" s="9"/>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="21" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="18" t="s">
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="15" t="s">
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
-      <c r="AF2" s="15"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="22" t="s">
+      <c r="E3" s="23"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="17" t="s">
+      <c r="H3" s="18"/>
+      <c r="I3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17" t="s">
+      <c r="J3" s="12"/>
+      <c r="K3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17" t="s">
+      <c r="L3" s="12"/>
+      <c r="M3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="17"/>
-      <c r="O3" s="27" t="s">
+      <c r="N3" s="12"/>
+      <c r="O3" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17" t="s">
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="9" t="s">
@@ -1246,20 +1380,20 @@
       </c>
       <c r="U3" s="9"/>
       <c r="V3" s="9"/>
-      <c r="W3" s="16" t="s">
+      <c r="W3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="X3" s="11" t="s">
         <v>21</v>
       </c>
       <c r="Y3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="20" t="s">
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AB3" s="20"/>
+      <c r="AB3" s="15"/>
       <c r="AC3" s="9" t="s">
         <v>17</v>
       </c>
@@ -1274,10 +1408,10 @@
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="20"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="1" t="s">
@@ -1306,15 +1440,15 @@
       <c r="V4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="W4" s="17"/>
-      <c r="X4" s="17"/>
-      <c r="Y4" s="1" t="s">
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="Z4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AA4" s="42" t="s">
         <v>15</v>
       </c>
       <c r="AB4" s="1" t="s">
@@ -1334,10 +1468,10 @@
       </c>
     </row>
     <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="9" t="s">
         <v>35</v>
       </c>
@@ -1346,11 +1480,11 @@
         <v>36</v>
       </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="25" t="s">
         <v>31</v>
       </c>
       <c r="H5" s="9"/>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="25" t="s">
         <v>37</v>
       </c>
       <c r="J5" s="9"/>
@@ -1366,25 +1500,45 @@
       <c r="N5" s="9">
         <v>3</v>
       </c>
-      <c r="O5" s="29">
+      <c r="O5" s="32">
         <f>L5*N5</f>
         <v>12</v>
       </c>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29" t="s">
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="R5" s="32"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
+      <c r="R5" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="U5" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="V5" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="W5" s="36">
+        <v>5</v>
+      </c>
+      <c r="X5" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="34"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -1397,31 +1551,39 @@
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="36"/>
+      <c r="X6" s="36"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="34"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9" t="s">
         <v>28</v>
       </c>
       <c r="F7" s="9"/>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="25" t="s">
         <v>30</v>
       </c>
       <c r="H7" s="9"/>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="25" t="s">
         <v>38</v>
       </c>
       <c r="J7" s="9"/>
@@ -1437,25 +1599,45 @@
       <c r="N7" s="9">
         <v>3</v>
       </c>
-      <c r="O7" s="29">
+      <c r="O7" s="32">
         <f t="shared" ref="O7" si="0">L7*N7</f>
         <v>9</v>
       </c>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29" t="s">
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="R7" s="33"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="34"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
+      <c r="R7" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="U7" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="V7" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="W7" s="35">
+        <v>3</v>
+      </c>
+      <c r="X7" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y7" s="34"/>
+      <c r="Z7" s="34"/>
+      <c r="AA7" s="34"/>
+      <c r="AB7" s="34"/>
+      <c r="AC7" s="34"/>
+      <c r="AD7" s="34"/>
+      <c r="AE7" s="34"/>
+      <c r="AF7" s="34"/>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="12"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -1468,33 +1650,41 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="33"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="34"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="35"/>
+      <c r="X8" s="39"/>
+      <c r="Y8" s="34"/>
+      <c r="Z8" s="34"/>
+      <c r="AA8" s="34"/>
+      <c r="AB8" s="34"/>
+      <c r="AC8" s="34"/>
+      <c r="AD8" s="34"/>
+      <c r="AE8" s="34"/>
+      <c r="AF8" s="34"/>
     </row>
     <row r="9" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="8" t="s">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8" t="s">
+      <c r="D9" s="25"/>
+      <c r="E9" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8" t="s">
+      <c r="F9" s="25"/>
+      <c r="G9" s="25" t="s">
         <v>39</v>
       </c>
       <c r="H9" s="9"/>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="25" t="s">
         <v>40</v>
       </c>
       <c r="J9" s="9"/>
@@ -1510,29 +1700,49 @@
       <c r="N9" s="9">
         <v>2</v>
       </c>
-      <c r="O9" s="29">
+      <c r="O9" s="32">
         <f t="shared" ref="O9" si="1">L9*N9</f>
         <v>8</v>
       </c>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29" t="s">
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="R9" s="33"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="34"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4"/>
+      <c r="R9" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="U9" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="V9" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="W9" s="35">
+        <v>3</v>
+      </c>
+      <c r="X9" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y9" s="34"/>
+      <c r="Z9" s="34"/>
+      <c r="AA9" s="34"/>
+      <c r="AB9" s="34"/>
+      <c r="AC9" s="34"/>
+      <c r="AD9" s="34"/>
+      <c r="AE9" s="34"/>
+      <c r="AF9" s="34"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -1541,31 +1751,39 @@
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="33"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="34"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="35"/>
+      <c r="X10" s="39"/>
+      <c r="Y10" s="34"/>
+      <c r="Z10" s="34"/>
+      <c r="AA10" s="34"/>
+      <c r="AB10" s="34"/>
+      <c r="AC10" s="34"/>
+      <c r="AD10" s="34"/>
+      <c r="AE10" s="34"/>
+      <c r="AF10" s="34"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
       <c r="E11" s="9" t="s">
         <v>28</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="25" t="s">
         <v>29</v>
       </c>
       <c r="H11" s="9"/>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="25" t="s">
         <v>41</v>
       </c>
       <c r="J11" s="9"/>
@@ -1581,27 +1799,47 @@
       <c r="N11" s="9">
         <v>3</v>
       </c>
-      <c r="O11" s="29">
+      <c r="O11" s="32">
         <f t="shared" ref="O11" si="2">L11*N11</f>
         <v>9</v>
       </c>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29" t="s">
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="R11" s="33"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="34"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
-      <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
+      <c r="R11" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="U11" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="V11" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="W11" s="36">
+        <v>5</v>
+      </c>
+      <c r="X11" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y11" s="34"/>
+      <c r="Z11" s="34"/>
+      <c r="AA11" s="34"/>
+      <c r="AB11" s="34"/>
+      <c r="AC11" s="34"/>
+      <c r="AD11" s="34"/>
+      <c r="AE11" s="34"/>
+      <c r="AF11" s="34"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -1612,33 +1850,41 @@
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="33"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="34"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="36"/>
+      <c r="X12" s="40"/>
+      <c r="Y12" s="34"/>
+      <c r="Z12" s="34"/>
+      <c r="AA12" s="34"/>
+      <c r="AB12" s="34"/>
+      <c r="AC12" s="34"/>
+      <c r="AD12" s="34"/>
+      <c r="AE12" s="34"/>
+      <c r="AF12" s="34"/>
     </row>
     <row r="13" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="8" t="s">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8" t="s">
+      <c r="D13" s="25"/>
+      <c r="E13" s="25" t="s">
         <v>44</v>
       </c>
       <c r="F13" s="9"/>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="25" t="s">
         <v>54</v>
       </c>
       <c r="H13" s="9"/>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="25" t="s">
         <v>49</v>
       </c>
       <c r="J13" s="9"/>
@@ -1654,27 +1900,47 @@
       <c r="N13" s="9">
         <v>3</v>
       </c>
-      <c r="O13" s="29">
+      <c r="O13" s="32">
         <f t="shared" ref="O13" si="3">L13*N13</f>
         <v>12</v>
       </c>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29" t="s">
+      <c r="P13" s="32"/>
+      <c r="Q13" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="R13" s="33"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="34"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
+      <c r="R13" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="U13" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="V13" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="W13" s="36">
+        <v>5</v>
+      </c>
+      <c r="X13" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y13" s="34"/>
+      <c r="Z13" s="34"/>
+      <c r="AA13" s="34"/>
+      <c r="AB13" s="34"/>
+      <c r="AC13" s="34"/>
+      <c r="AD13" s="34"/>
+      <c r="AE13" s="34"/>
+      <c r="AF13" s="34"/>
     </row>
     <row r="14" spans="1:32" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -1685,31 +1951,39 @@
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="33"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="34"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
-      <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="36"/>
+      <c r="X14" s="40"/>
+      <c r="Y14" s="34"/>
+      <c r="Z14" s="34"/>
+      <c r="AA14" s="34"/>
+      <c r="AB14" s="34"/>
+      <c r="AC14" s="34"/>
+      <c r="AD14" s="34"/>
+      <c r="AE14" s="34"/>
+      <c r="AF14" s="34"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
       <c r="E15" s="9" t="s">
         <v>43</v>
       </c>
       <c r="F15" s="9"/>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="25" t="s">
         <v>55</v>
       </c>
       <c r="H15" s="9"/>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="25" t="s">
         <v>22</v>
       </c>
       <c r="J15" s="9"/>
@@ -1725,27 +1999,47 @@
       <c r="N15" s="9">
         <v>3</v>
       </c>
-      <c r="O15" s="30">
+      <c r="O15" s="35">
         <f t="shared" ref="O15" si="4">L15*N15</f>
         <v>6</v>
       </c>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30" t="s">
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="R15" s="33"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="34"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
+      <c r="R15" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="U15" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="V15" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="W15" s="37">
+        <v>4</v>
+      </c>
+      <c r="X15" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y15" s="34"/>
+      <c r="Z15" s="34"/>
+      <c r="AA15" s="34"/>
+      <c r="AB15" s="34"/>
+      <c r="AC15" s="34"/>
+      <c r="AD15" s="34"/>
+      <c r="AE15" s="34"/>
+      <c r="AF15" s="34"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -1756,35 +2050,43 @@
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="30"/>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="33"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="34"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
+      <c r="O16" s="35"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="35"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="37"/>
+      <c r="X16" s="37"/>
+      <c r="Y16" s="34"/>
+      <c r="Z16" s="34"/>
+      <c r="AA16" s="34"/>
+      <c r="AB16" s="34"/>
+      <c r="AC16" s="34"/>
+      <c r="AD16" s="34"/>
+      <c r="AE16" s="34"/>
+      <c r="AF16" s="34"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="9"/>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="8"/>
+      <c r="D17" s="25"/>
       <c r="E17" s="9" t="s">
         <v>48</v>
       </c>
       <c r="F17" s="9"/>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="25" t="s">
         <v>56</v>
       </c>
       <c r="H17" s="9"/>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="25" t="s">
         <v>23</v>
       </c>
       <c r="J17" s="9"/>
@@ -1800,27 +2102,47 @@
       <c r="N17" s="9">
         <v>3</v>
       </c>
-      <c r="O17" s="30">
+      <c r="O17" s="35">
         <f t="shared" ref="O17" si="5">L17*N17</f>
         <v>6</v>
       </c>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="30" t="s">
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="R17" s="33"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="34"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
+      <c r="R17" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="U17" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="V17" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="W17" s="37">
+        <v>4</v>
+      </c>
+      <c r="X17" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y17" s="34"/>
+      <c r="Z17" s="34"/>
+      <c r="AA17" s="34"/>
+      <c r="AB17" s="34"/>
+      <c r="AC17" s="34"/>
+      <c r="AD17" s="34"/>
+      <c r="AE17" s="34"/>
+      <c r="AF17" s="34"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -1831,31 +2153,39 @@
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="33"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="34"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="37"/>
+      <c r="X18" s="37"/>
+      <c r="Y18" s="34"/>
+      <c r="Z18" s="34"/>
+      <c r="AA18" s="34"/>
+      <c r="AB18" s="34"/>
+      <c r="AC18" s="34"/>
+      <c r="AD18" s="34"/>
+      <c r="AE18" s="34"/>
+      <c r="AF18" s="34"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
       <c r="E19" s="9" t="s">
         <v>45</v>
       </c>
       <c r="F19" s="9"/>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="25" t="s">
         <v>57</v>
       </c>
       <c r="H19" s="9"/>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="25" t="s">
         <v>50</v>
       </c>
       <c r="J19" s="9"/>
@@ -1871,27 +2201,47 @@
       <c r="N19" s="9">
         <v>2</v>
       </c>
-      <c r="O19" s="29">
+      <c r="O19" s="32">
         <f t="shared" ref="O19" si="6">L19*N19</f>
         <v>8</v>
       </c>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="29" t="s">
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="R19" s="33"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="34"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
-      <c r="X19" s="4"/>
+      <c r="R19" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="U19" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="V19" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="W19" s="38">
+        <v>2</v>
+      </c>
+      <c r="X19" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y19" s="34"/>
+      <c r="Z19" s="34"/>
+      <c r="AA19" s="34"/>
+      <c r="AB19" s="34"/>
+      <c r="AC19" s="34"/>
+      <c r="AD19" s="34"/>
+      <c r="AE19" s="34"/>
+      <c r="AF19" s="34"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -1902,35 +2252,43 @@
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="33"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="34"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="38"/>
+      <c r="X20" s="38"/>
+      <c r="Y20" s="34"/>
+      <c r="Z20" s="34"/>
+      <c r="AA20" s="34"/>
+      <c r="AB20" s="34"/>
+      <c r="AC20" s="34"/>
+      <c r="AD20" s="34"/>
+      <c r="AE20" s="34"/>
+      <c r="AF20" s="34"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="9"/>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="8"/>
+      <c r="D21" s="25"/>
       <c r="E21" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F21" s="9"/>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="25" t="s">
         <v>58</v>
       </c>
       <c r="H21" s="9"/>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="25" t="s">
         <v>24</v>
       </c>
       <c r="J21" s="9"/>
@@ -1946,27 +2304,47 @@
       <c r="N21" s="9">
         <v>4</v>
       </c>
-      <c r="O21" s="31">
+      <c r="O21" s="33">
         <f t="shared" ref="O21" si="7">L21*N21</f>
         <v>16</v>
       </c>
-      <c r="P21" s="31"/>
-      <c r="Q21" s="31" t="s">
+      <c r="P21" s="33"/>
+      <c r="Q21" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="R21" s="33"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="34"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
+      <c r="R21" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="U21" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="V21" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="W21" s="36">
+        <v>5</v>
+      </c>
+      <c r="X21" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y21" s="34"/>
+      <c r="Z21" s="34"/>
+      <c r="AA21" s="34"/>
+      <c r="AB21" s="34"/>
+      <c r="AC21" s="34"/>
+      <c r="AD21" s="34"/>
+      <c r="AE21" s="34"/>
+      <c r="AF21" s="34"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -1977,31 +2355,39 @@
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="31"/>
-      <c r="Q22" s="31"/>
-      <c r="R22" s="33"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="34"/>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-      <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="33"/>
+      <c r="Q22" s="33"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="36"/>
+      <c r="X22" s="36"/>
+      <c r="Y22" s="34"/>
+      <c r="Z22" s="34"/>
+      <c r="AA22" s="34"/>
+      <c r="AB22" s="34"/>
+      <c r="AC22" s="34"/>
+      <c r="AD22" s="34"/>
+      <c r="AE22" s="34"/>
+      <c r="AF22" s="34"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
       <c r="E23" s="9" t="s">
         <v>27</v>
       </c>
       <c r="F23" s="9"/>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="25" t="s">
         <v>58</v>
       </c>
       <c r="H23" s="9"/>
-      <c r="I23" s="8" t="s">
+      <c r="I23" s="25" t="s">
         <v>51</v>
       </c>
       <c r="J23" s="9"/>
@@ -2017,27 +2403,47 @@
       <c r="N23" s="9">
         <v>4</v>
       </c>
-      <c r="O23" s="31">
+      <c r="O23" s="33">
         <f t="shared" ref="O23" si="8">L23*N23</f>
         <v>16</v>
       </c>
-      <c r="P23" s="31"/>
-      <c r="Q23" s="31" t="s">
+      <c r="P23" s="33"/>
+      <c r="Q23" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="R23" s="33"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="34"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="4"/>
+      <c r="R23" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="U23" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="V23" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="W23" s="37">
+        <v>4</v>
+      </c>
+      <c r="X23" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y23" s="34"/>
+      <c r="Z23" s="34"/>
+      <c r="AA23" s="34"/>
+      <c r="AB23" s="34"/>
+      <c r="AC23" s="34"/>
+      <c r="AD23" s="34"/>
+      <c r="AE23" s="34"/>
+      <c r="AF23" s="34"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -2048,102 +2454,184 @@
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="31"/>
-      <c r="Q24" s="31"/>
-      <c r="R24" s="33"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="34"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="33"/>
+      <c r="Q24" s="33"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="37"/>
+      <c r="X24" s="37"/>
+      <c r="Y24" s="34"/>
+      <c r="Z24" s="34"/>
+      <c r="AA24" s="34"/>
+      <c r="AB24" s="34"/>
+      <c r="AC24" s="34"/>
+      <c r="AD24" s="34"/>
+      <c r="AE24" s="34"/>
+      <c r="AF24" s="34"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="178">
-    <mergeCell ref="W21:W22"/>
-    <mergeCell ref="W23:W24"/>
-    <mergeCell ref="X5:X6"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="X15:X16"/>
-    <mergeCell ref="X17:X18"/>
-    <mergeCell ref="X19:X20"/>
-    <mergeCell ref="X21:X22"/>
-    <mergeCell ref="X23:X24"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="W5:W6"/>
-    <mergeCell ref="W7:W8"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="W11:W12"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="W15:W16"/>
-    <mergeCell ref="W17:W18"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="U23:U24"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="V11:V12"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="V15:V16"/>
-    <mergeCell ref="V17:V18"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="V21:V22"/>
-    <mergeCell ref="V23:V24"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="U11:U12"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="U15:U16"/>
-    <mergeCell ref="U17:U18"/>
-    <mergeCell ref="U19:U20"/>
-    <mergeCell ref="U21:U22"/>
-    <mergeCell ref="R23:S24"/>
-    <mergeCell ref="T5:T6"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="T11:T12"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="T17:T18"/>
-    <mergeCell ref="T19:T20"/>
-    <mergeCell ref="T21:T22"/>
-    <mergeCell ref="T23:T24"/>
-    <mergeCell ref="R5:S6"/>
-    <mergeCell ref="R7:S8"/>
-    <mergeCell ref="R9:S10"/>
-    <mergeCell ref="R11:S12"/>
-    <mergeCell ref="R13:S14"/>
-    <mergeCell ref="R15:S16"/>
-    <mergeCell ref="R17:S18"/>
-    <mergeCell ref="R19:S20"/>
-    <mergeCell ref="R21:S22"/>
-    <mergeCell ref="A2:B4"/>
-    <mergeCell ref="C2:D4"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="Y2:AF2"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="R2:X2"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="R3:S4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="G2:Q2"/>
-    <mergeCell ref="G3:H4"/>
-    <mergeCell ref="O3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="I3:J4"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="E2:F4"/>
+  <mergeCells count="258">
+    <mergeCell ref="AA21:AA22"/>
+    <mergeCell ref="AB21:AB22"/>
+    <mergeCell ref="AC21:AC22"/>
+    <mergeCell ref="AD21:AD22"/>
+    <mergeCell ref="AE21:AE22"/>
+    <mergeCell ref="AF21:AF22"/>
+    <mergeCell ref="AA23:AA24"/>
+    <mergeCell ref="AB23:AB24"/>
+    <mergeCell ref="AC23:AC24"/>
+    <mergeCell ref="AD23:AD24"/>
+    <mergeCell ref="AE23:AE24"/>
+    <mergeCell ref="AF23:AF24"/>
+    <mergeCell ref="AA17:AA18"/>
+    <mergeCell ref="AB17:AB18"/>
+    <mergeCell ref="AC17:AC18"/>
+    <mergeCell ref="AD17:AD18"/>
+    <mergeCell ref="AE17:AE18"/>
+    <mergeCell ref="AF17:AF18"/>
+    <mergeCell ref="AA19:AA20"/>
+    <mergeCell ref="AB19:AB20"/>
+    <mergeCell ref="AC19:AC20"/>
+    <mergeCell ref="AD19:AD20"/>
+    <mergeCell ref="AE19:AE20"/>
+    <mergeCell ref="AF19:AF20"/>
+    <mergeCell ref="AA13:AA14"/>
+    <mergeCell ref="AB13:AB14"/>
+    <mergeCell ref="AC13:AC14"/>
+    <mergeCell ref="AD13:AD14"/>
+    <mergeCell ref="AE13:AE14"/>
+    <mergeCell ref="AF13:AF14"/>
+    <mergeCell ref="AA15:AA16"/>
+    <mergeCell ref="AB15:AB16"/>
+    <mergeCell ref="AC15:AC16"/>
+    <mergeCell ref="AD15:AD16"/>
+    <mergeCell ref="AE15:AE16"/>
+    <mergeCell ref="AF15:AF16"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AA11:AA12"/>
+    <mergeCell ref="AB11:AB12"/>
+    <mergeCell ref="AC11:AC12"/>
+    <mergeCell ref="AD11:AD12"/>
+    <mergeCell ref="AE11:AE12"/>
+    <mergeCell ref="AF11:AF12"/>
+    <mergeCell ref="AA5:AA6"/>
+    <mergeCell ref="AB5:AB6"/>
+    <mergeCell ref="AC5:AC6"/>
+    <mergeCell ref="AD5:AD6"/>
+    <mergeCell ref="AE5:AE6"/>
+    <mergeCell ref="AF5:AF6"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="AC7:AC8"/>
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="AE7:AE8"/>
+    <mergeCell ref="AF7:AF8"/>
+    <mergeCell ref="Y23:Y24"/>
+    <mergeCell ref="Z5:Z6"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="Z11:Z12"/>
+    <mergeCell ref="Z13:Z14"/>
+    <mergeCell ref="Z15:Z16"/>
+    <mergeCell ref="Z17:Z18"/>
+    <mergeCell ref="Z19:Z20"/>
+    <mergeCell ref="Z21:Z22"/>
+    <mergeCell ref="Z23:Z24"/>
+    <mergeCell ref="Y5:Y6"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Y11:Y12"/>
+    <mergeCell ref="Y13:Y14"/>
+    <mergeCell ref="Y15:Y16"/>
+    <mergeCell ref="Y17:Y18"/>
+    <mergeCell ref="Y19:Y20"/>
+    <mergeCell ref="Y21:Y22"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="Q17:Q18"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="Q21:Q22"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="O5:P6"/>
+    <mergeCell ref="O7:P8"/>
+    <mergeCell ref="O9:P10"/>
+    <mergeCell ref="O11:P12"/>
+    <mergeCell ref="O13:P14"/>
+    <mergeCell ref="O15:P16"/>
+    <mergeCell ref="O17:P18"/>
+    <mergeCell ref="O19:P20"/>
+    <mergeCell ref="O21:P22"/>
+    <mergeCell ref="O23:P24"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="G17:H18"/>
+    <mergeCell ref="G19:H20"/>
+    <mergeCell ref="G21:H22"/>
+    <mergeCell ref="G23:H24"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="G9:H10"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="E13:F14"/>
+    <mergeCell ref="E21:F22"/>
+    <mergeCell ref="E23:F24"/>
+    <mergeCell ref="E9:F10"/>
+    <mergeCell ref="E11:F12"/>
+    <mergeCell ref="E15:F16"/>
     <mergeCell ref="E17:F18"/>
     <mergeCell ref="E19:F20"/>
     <mergeCell ref="A21:B24"/>
@@ -2168,82 +2656,89 @@
     <mergeCell ref="I9:J10"/>
     <mergeCell ref="I11:J12"/>
     <mergeCell ref="G15:H16"/>
-    <mergeCell ref="G17:H18"/>
-    <mergeCell ref="G19:H20"/>
-    <mergeCell ref="G21:H22"/>
-    <mergeCell ref="G23:H24"/>
-    <mergeCell ref="G7:H8"/>
-    <mergeCell ref="G9:H10"/>
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="E13:F14"/>
-    <mergeCell ref="E21:F22"/>
-    <mergeCell ref="E23:F24"/>
-    <mergeCell ref="E9:F10"/>
-    <mergeCell ref="E11:F12"/>
-    <mergeCell ref="E15:F16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="O5:P6"/>
-    <mergeCell ref="O7:P8"/>
-    <mergeCell ref="O9:P10"/>
-    <mergeCell ref="O11:P12"/>
-    <mergeCell ref="O13:P14"/>
-    <mergeCell ref="O15:P16"/>
-    <mergeCell ref="O17:P18"/>
-    <mergeCell ref="O19:P20"/>
-    <mergeCell ref="O21:P22"/>
-    <mergeCell ref="O23:P24"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M23:M24"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="Q17:Q18"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="Q21:Q22"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="A2:B4"/>
+    <mergeCell ref="C2:D4"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="Y2:AF2"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="R2:X2"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="R3:S4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="G2:Q2"/>
+    <mergeCell ref="G3:H4"/>
+    <mergeCell ref="O3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="I3:J4"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="E2:F4"/>
+    <mergeCell ref="R23:S24"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="T17:T18"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="T21:T22"/>
+    <mergeCell ref="T23:T24"/>
+    <mergeCell ref="R5:S6"/>
+    <mergeCell ref="R7:S8"/>
+    <mergeCell ref="R9:S10"/>
+    <mergeCell ref="R11:S12"/>
+    <mergeCell ref="R13:S14"/>
+    <mergeCell ref="R15:S16"/>
+    <mergeCell ref="R17:S18"/>
+    <mergeCell ref="R19:S20"/>
+    <mergeCell ref="R21:S22"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="U15:U16"/>
+    <mergeCell ref="U17:U18"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="U21:U22"/>
+    <mergeCell ref="U23:U24"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="V11:V12"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="V15:V16"/>
+    <mergeCell ref="V17:V18"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="V21:V22"/>
+    <mergeCell ref="V23:V24"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="W7:W8"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="W11:W12"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="W15:W16"/>
+    <mergeCell ref="W17:W18"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:W22"/>
+    <mergeCell ref="W23:W24"/>
+    <mergeCell ref="X5:X6"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="X15:X16"/>
+    <mergeCell ref="X17:X18"/>
+    <mergeCell ref="X19:X20"/>
+    <mergeCell ref="X21:X22"/>
+    <mergeCell ref="X23:X24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2254,7 +2749,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="M16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="M28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se termina Matriz de Riesgo PEP
</commit_message>
<xml_diff>
--- a/trabajos.inacap.2019/Preparacion y evaluacion de proyecto (PEP)/Acumulado/Matriz de Riesgo.xlsx
+++ b/trabajos.inacap.2019/Preparacion y evaluacion de proyecto (PEP)/Acumulado/Matriz de Riesgo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\GitHub INACAP\inacap.2019\trabajos.inacap.2019\Preparacion y evaluacion de proyecto (PEP)\Acumulado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E42AE4-25F1-4521-993E-4100D65DE316}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE98E851-A686-4A9E-9E45-2AA83EF81628}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="95">
   <si>
     <t>Procesos</t>
   </si>
@@ -326,6 +326,21 @@
   </si>
   <si>
     <t>Regular</t>
+  </si>
+  <si>
+    <t>Menor</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Mayor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valor </t>
+  </si>
+  <si>
+    <t>Medias</t>
   </si>
 </sst>
 </file>
@@ -348,7 +363,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,6 +415,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -566,21 +587,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -626,39 +668,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -668,16 +677,16 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1274,8 +1283,8 @@
   </sheetPr>
   <dimension ref="A2:AF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AB23" sqref="AB23:AB24"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AE17" sqref="AE17:AE24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,71 +1313,71 @@
         <v>1</v>
       </c>
       <c r="D2" s="9"/>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="16" t="s">
+      <c r="F2" s="29"/>
+      <c r="G2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="13" t="s">
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="10" t="s">
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17"/>
+      <c r="AE2" s="17"/>
+      <c r="AF2" s="17"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="17" t="s">
+      <c r="E3" s="30"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="12" t="s">
+      <c r="H3" s="25"/>
+      <c r="I3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12" t="s">
+      <c r="J3" s="19"/>
+      <c r="K3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12" t="s">
+      <c r="L3" s="19"/>
+      <c r="M3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="12"/>
-      <c r="O3" s="21" t="s">
+      <c r="N3" s="19"/>
+      <c r="O3" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12" t="s">
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="9" t="s">
@@ -1380,20 +1389,20 @@
       </c>
       <c r="U3" s="9"/>
       <c r="V3" s="9"/>
-      <c r="W3" s="11" t="s">
+      <c r="W3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="X3" s="11" t="s">
+      <c r="X3" s="18" t="s">
         <v>21</v>
       </c>
       <c r="Y3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="15" t="s">
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="AB3" s="15"/>
+      <c r="AB3" s="22"/>
       <c r="AC3" s="9" t="s">
         <v>17</v>
       </c>
@@ -1408,10 +1417,10 @@
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="20"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="1" t="s">
@@ -1440,38 +1449,38 @@
       <c r="V4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="41" t="s">
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Z4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA4" s="42" t="s">
+      <c r="AA4" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC4" s="1" t="s">
+      <c r="AC4" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AD4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AE4" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF4" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="AF4" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="27"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="9" t="s">
         <v>35</v>
       </c>
@@ -1480,11 +1489,11 @@
         <v>36</v>
       </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="10" t="s">
         <v>31</v>
       </c>
       <c r="H5" s="9"/>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="10" t="s">
         <v>37</v>
       </c>
       <c r="J5" s="9"/>
@@ -1500,15 +1509,15 @@
       <c r="N5" s="9">
         <v>3</v>
       </c>
-      <c r="O5" s="32">
+      <c r="O5" s="35">
         <f>L5*N5</f>
         <v>12</v>
       </c>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32" t="s">
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="R5" s="25" t="s">
+      <c r="R5" s="10" t="s">
         <v>68</v>
       </c>
       <c r="S5" s="9"/>
@@ -1521,24 +1530,42 @@
       <c r="V5" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="W5" s="36">
+      <c r="W5" s="32">
         <v>5</v>
       </c>
-      <c r="X5" s="36" t="s">
+      <c r="X5" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="34"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="6"/>
+      <c r="Y5" s="32">
+        <v>2.4</v>
+      </c>
+      <c r="Z5" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA5" s="32">
+        <v>2.4</v>
+      </c>
+      <c r="AB5" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC5" s="36">
+        <f>(AA5+AA7)/2</f>
+        <v>2.7</v>
+      </c>
+      <c r="AD5" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE5" s="37">
+        <f>(AC5+AC9+AC13)/3</f>
+        <v>2.2950000000000004</v>
+      </c>
+      <c r="AF5" s="32" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -1551,39 +1578,39 @@
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="35"/>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
       <c r="T6" s="9"/>
       <c r="U6" s="9"/>
       <c r="V6" s="9"/>
-      <c r="W6" s="36"/>
-      <c r="X6" s="36"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="34"/>
-      <c r="AA6" s="5"/>
-      <c r="AB6" s="5"/>
-      <c r="AC6" s="5"/>
-      <c r="AD6" s="5"/>
-      <c r="AE6" s="5"/>
-      <c r="AF6" s="5"/>
+      <c r="W6" s="32"/>
+      <c r="X6" s="32"/>
+      <c r="Y6" s="32"/>
+      <c r="Z6" s="32"/>
+      <c r="AA6" s="32"/>
+      <c r="AB6" s="32"/>
+      <c r="AC6" s="36"/>
+      <c r="AD6" s="32"/>
+      <c r="AE6" s="37"/>
+      <c r="AF6" s="32"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="29"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9" t="s">
         <v>28</v>
       </c>
       <c r="F7" s="9"/>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="10" t="s">
         <v>30</v>
       </c>
       <c r="H7" s="9"/>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="10" t="s">
         <v>38</v>
       </c>
       <c r="J7" s="9"/>
@@ -1599,15 +1626,15 @@
       <c r="N7" s="9">
         <v>3</v>
       </c>
-      <c r="O7" s="32">
+      <c r="O7" s="35">
         <f t="shared" ref="O7" si="0">L7*N7</f>
         <v>9</v>
       </c>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32" t="s">
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="R7" s="25" t="s">
+      <c r="R7" s="10" t="s">
         <v>67</v>
       </c>
       <c r="S7" s="9"/>
@@ -1620,24 +1647,32 @@
       <c r="V7" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="W7" s="35">
+      <c r="W7" s="7">
         <v>3</v>
       </c>
-      <c r="X7" s="39" t="s">
+      <c r="X7" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="Y7" s="34"/>
-      <c r="Z7" s="34"/>
-      <c r="AA7" s="34"/>
-      <c r="AB7" s="34"/>
-      <c r="AC7" s="34"/>
-      <c r="AD7" s="34"/>
-      <c r="AE7" s="34"/>
-      <c r="AF7" s="34"/>
+      <c r="Y7" s="7">
+        <v>3</v>
+      </c>
+      <c r="Z7" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA7" s="7">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC7" s="36"/>
+      <c r="AD7" s="32"/>
+      <c r="AE7" s="37"/>
+      <c r="AF7" s="32"/>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -1650,41 +1685,41 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
       <c r="R8" s="9"/>
       <c r="S8" s="9"/>
       <c r="T8" s="9"/>
       <c r="U8" s="9"/>
       <c r="V8" s="9"/>
-      <c r="W8" s="35"/>
-      <c r="X8" s="39"/>
-      <c r="Y8" s="34"/>
-      <c r="Z8" s="34"/>
-      <c r="AA8" s="34"/>
-      <c r="AB8" s="34"/>
-      <c r="AC8" s="34"/>
-      <c r="AD8" s="34"/>
-      <c r="AE8" s="34"/>
-      <c r="AF8" s="34"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="36"/>
+      <c r="AD8" s="32"/>
+      <c r="AE8" s="37"/>
+      <c r="AF8" s="32"/>
     </row>
     <row r="9" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="25" t="s">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25" t="s">
+      <c r="D9" s="10"/>
+      <c r="E9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10" t="s">
         <v>39</v>
       </c>
       <c r="H9" s="9"/>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="10" t="s">
         <v>40</v>
       </c>
       <c r="J9" s="9"/>
@@ -1700,15 +1735,15 @@
       <c r="N9" s="9">
         <v>2</v>
       </c>
-      <c r="O9" s="32">
+      <c r="O9" s="35">
         <f t="shared" ref="O9" si="1">L9*N9</f>
         <v>8</v>
       </c>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32" t="s">
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="R9" s="25" t="s">
+      <c r="R9" s="10" t="s">
         <v>72</v>
       </c>
       <c r="S9" s="9"/>
@@ -1721,28 +1756,41 @@
       <c r="V9" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="W9" s="35">
+      <c r="W9" s="7">
         <v>3</v>
       </c>
-      <c r="X9" s="39" t="s">
+      <c r="X9" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="Y9" s="34"/>
-      <c r="Z9" s="34"/>
-      <c r="AA9" s="34"/>
-      <c r="AB9" s="34"/>
-      <c r="AC9" s="34"/>
-      <c r="AD9" s="34"/>
-      <c r="AE9" s="34"/>
-      <c r="AF9" s="34"/>
+      <c r="Y9" s="32">
+        <v>2.67</v>
+      </c>
+      <c r="Z9" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA9" s="32">
+        <v>2.67</v>
+      </c>
+      <c r="AB9" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC9" s="37">
+        <f>(AA9+AA11)/2</f>
+        <v>2.2349999999999999</v>
+      </c>
+      <c r="AD9" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE9" s="37"/>
+      <c r="AF9" s="32"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -1751,39 +1799,39 @@
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
       <c r="T10" s="9"/>
       <c r="U10" s="9"/>
       <c r="V10" s="9"/>
-      <c r="W10" s="35"/>
-      <c r="X10" s="39"/>
-      <c r="Y10" s="34"/>
-      <c r="Z10" s="34"/>
-      <c r="AA10" s="34"/>
-      <c r="AB10" s="34"/>
-      <c r="AC10" s="34"/>
-      <c r="AD10" s="34"/>
-      <c r="AE10" s="34"/>
-      <c r="AF10" s="34"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="32"/>
+      <c r="Z10" s="32"/>
+      <c r="AA10" s="32"/>
+      <c r="AB10" s="32"/>
+      <c r="AC10" s="37"/>
+      <c r="AD10" s="32"/>
+      <c r="AE10" s="37"/>
+      <c r="AF10" s="32"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="9" t="s">
         <v>28</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="10" t="s">
         <v>29</v>
       </c>
       <c r="H11" s="9"/>
-      <c r="I11" s="25" t="s">
+      <c r="I11" s="10" t="s">
         <v>41</v>
       </c>
       <c r="J11" s="9"/>
@@ -1799,15 +1847,15 @@
       <c r="N11" s="9">
         <v>3</v>
       </c>
-      <c r="O11" s="32">
+      <c r="O11" s="35">
         <f t="shared" ref="O11" si="2">L11*N11</f>
         <v>9</v>
       </c>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="32" t="s">
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="R11" s="25" t="s">
+      <c r="R11" s="10" t="s">
         <v>69</v>
       </c>
       <c r="S11" s="9"/>
@@ -1820,26 +1868,34 @@
       <c r="V11" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="W11" s="36">
+      <c r="W11" s="32">
         <v>5</v>
       </c>
-      <c r="X11" s="40" t="s">
+      <c r="X11" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="Y11" s="34"/>
-      <c r="Z11" s="34"/>
-      <c r="AA11" s="34"/>
-      <c r="AB11" s="34"/>
-      <c r="AC11" s="34"/>
-      <c r="AD11" s="34"/>
-      <c r="AE11" s="34"/>
-      <c r="AF11" s="34"/>
+      <c r="Y11" s="32">
+        <v>1.8</v>
+      </c>
+      <c r="Z11" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA11" s="32">
+        <v>1.8</v>
+      </c>
+      <c r="AB11" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC11" s="37"/>
+      <c r="AD11" s="32"/>
+      <c r="AE11" s="37"/>
+      <c r="AF11" s="32"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -1850,41 +1906,41 @@
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
-      <c r="Q12" s="32"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="35"/>
       <c r="R12" s="9"/>
       <c r="S12" s="9"/>
       <c r="T12" s="9"/>
       <c r="U12" s="9"/>
       <c r="V12" s="9"/>
-      <c r="W12" s="36"/>
-      <c r="X12" s="40"/>
-      <c r="Y12" s="34"/>
-      <c r="Z12" s="34"/>
-      <c r="AA12" s="34"/>
-      <c r="AB12" s="34"/>
-      <c r="AC12" s="34"/>
-      <c r="AD12" s="34"/>
-      <c r="AE12" s="34"/>
-      <c r="AF12" s="34"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="32"/>
+      <c r="AA12" s="32"/>
+      <c r="AB12" s="32"/>
+      <c r="AC12" s="37"/>
+      <c r="AD12" s="32"/>
+      <c r="AE12" s="37"/>
+      <c r="AF12" s="32"/>
     </row>
     <row r="13" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="25" t="s">
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25" t="s">
+      <c r="D13" s="10"/>
+      <c r="E13" s="10" t="s">
         <v>44</v>
       </c>
       <c r="F13" s="9"/>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="10" t="s">
         <v>54</v>
       </c>
       <c r="H13" s="9"/>
-      <c r="I13" s="25" t="s">
+      <c r="I13" s="10" t="s">
         <v>49</v>
       </c>
       <c r="J13" s="9"/>
@@ -1900,15 +1956,15 @@
       <c r="N13" s="9">
         <v>3</v>
       </c>
-      <c r="O13" s="32">
+      <c r="O13" s="35">
         <f t="shared" ref="O13" si="3">L13*N13</f>
         <v>12</v>
       </c>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32" t="s">
+      <c r="P13" s="35"/>
+      <c r="Q13" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="R13" s="25" t="s">
+      <c r="R13" s="10" t="s">
         <v>70</v>
       </c>
       <c r="S13" s="9"/>
@@ -1921,26 +1977,39 @@
       <c r="V13" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="W13" s="36">
+      <c r="W13" s="32">
         <v>5</v>
       </c>
-      <c r="X13" s="40" t="s">
+      <c r="X13" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="Y13" s="34"/>
-      <c r="Z13" s="34"/>
-      <c r="AA13" s="34"/>
-      <c r="AB13" s="34"/>
-      <c r="AC13" s="34"/>
-      <c r="AD13" s="34"/>
-      <c r="AE13" s="34"/>
-      <c r="AF13" s="34"/>
+      <c r="Y13" s="32">
+        <v>2.4</v>
+      </c>
+      <c r="Z13" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA13" s="32">
+        <v>2.4</v>
+      </c>
+      <c r="AB13" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC13" s="32">
+        <f>(AA13+AA15)/2</f>
+        <v>1.95</v>
+      </c>
+      <c r="AD13" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE13" s="37"/>
+      <c r="AF13" s="32"/>
     </row>
     <row r="14" spans="1:32" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -1951,39 +2020,39 @@
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
       <c r="R14" s="9"/>
       <c r="S14" s="9"/>
       <c r="T14" s="9"/>
       <c r="U14" s="9"/>
       <c r="V14" s="9"/>
-      <c r="W14" s="36"/>
-      <c r="X14" s="40"/>
-      <c r="Y14" s="34"/>
-      <c r="Z14" s="34"/>
-      <c r="AA14" s="34"/>
-      <c r="AB14" s="34"/>
-      <c r="AC14" s="34"/>
-      <c r="AD14" s="34"/>
-      <c r="AE14" s="34"/>
-      <c r="AF14" s="34"/>
+      <c r="W14" s="32"/>
+      <c r="X14" s="32"/>
+      <c r="Y14" s="32"/>
+      <c r="Z14" s="32"/>
+      <c r="AA14" s="32"/>
+      <c r="AB14" s="32"/>
+      <c r="AC14" s="32"/>
+      <c r="AD14" s="32"/>
+      <c r="AE14" s="37"/>
+      <c r="AF14" s="32"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="9" t="s">
         <v>43</v>
       </c>
       <c r="F15" s="9"/>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="10" t="s">
         <v>55</v>
       </c>
       <c r="H15" s="9"/>
-      <c r="I15" s="25" t="s">
+      <c r="I15" s="10" t="s">
         <v>22</v>
       </c>
       <c r="J15" s="9"/>
@@ -1999,15 +2068,15 @@
       <c r="N15" s="9">
         <v>3</v>
       </c>
-      <c r="O15" s="35">
+      <c r="O15" s="7">
         <f t="shared" ref="O15" si="4">L15*N15</f>
         <v>6</v>
       </c>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35" t="s">
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="R15" s="25" t="s">
+      <c r="R15" s="10" t="s">
         <v>71</v>
       </c>
       <c r="S15" s="9"/>
@@ -2020,26 +2089,34 @@
       <c r="V15" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="W15" s="37">
+      <c r="W15" s="33">
         <v>4</v>
       </c>
-      <c r="X15" s="37" t="s">
+      <c r="X15" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="Y15" s="34"/>
-      <c r="Z15" s="34"/>
-      <c r="AA15" s="34"/>
-      <c r="AB15" s="34"/>
-      <c r="AC15" s="34"/>
-      <c r="AD15" s="34"/>
-      <c r="AE15" s="34"/>
-      <c r="AF15" s="34"/>
+      <c r="Y15" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="Z15" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA15" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="AB15" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC15" s="32"/>
+      <c r="AD15" s="32"/>
+      <c r="AE15" s="37"/>
+      <c r="AF15" s="32"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -2050,43 +2127,43 @@
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
       <c r="R16" s="9"/>
       <c r="S16" s="9"/>
       <c r="T16" s="9"/>
       <c r="U16" s="9"/>
       <c r="V16" s="9"/>
-      <c r="W16" s="37"/>
-      <c r="X16" s="37"/>
-      <c r="Y16" s="34"/>
-      <c r="Z16" s="34"/>
-      <c r="AA16" s="34"/>
-      <c r="AB16" s="34"/>
-      <c r="AC16" s="34"/>
-      <c r="AD16" s="34"/>
-      <c r="AE16" s="34"/>
-      <c r="AF16" s="34"/>
+      <c r="W16" s="33"/>
+      <c r="X16" s="33"/>
+      <c r="Y16" s="32"/>
+      <c r="Z16" s="32"/>
+      <c r="AA16" s="32"/>
+      <c r="AB16" s="32"/>
+      <c r="AC16" s="32"/>
+      <c r="AD16" s="32"/>
+      <c r="AE16" s="37"/>
+      <c r="AF16" s="32"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="9"/>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="25"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="9" t="s">
         <v>48</v>
       </c>
       <c r="F17" s="9"/>
-      <c r="G17" s="25" t="s">
+      <c r="G17" s="10" t="s">
         <v>56</v>
       </c>
       <c r="H17" s="9"/>
-      <c r="I17" s="25" t="s">
+      <c r="I17" s="10" t="s">
         <v>23</v>
       </c>
       <c r="J17" s="9"/>
@@ -2102,15 +2179,15 @@
       <c r="N17" s="9">
         <v>3</v>
       </c>
-      <c r="O17" s="35">
+      <c r="O17" s="7">
         <f t="shared" ref="O17" si="5">L17*N17</f>
         <v>6</v>
       </c>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35" t="s">
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="R17" s="25" t="s">
+      <c r="R17" s="10" t="s">
         <v>73</v>
       </c>
       <c r="S17" s="9"/>
@@ -2123,26 +2200,44 @@
       <c r="V17" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="W17" s="37">
+      <c r="W17" s="33">
         <v>4</v>
       </c>
-      <c r="X17" s="37" t="s">
+      <c r="X17" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="Y17" s="34"/>
-      <c r="Z17" s="34"/>
-      <c r="AA17" s="34"/>
-      <c r="AB17" s="34"/>
-      <c r="AC17" s="34"/>
-      <c r="AD17" s="34"/>
-      <c r="AE17" s="34"/>
-      <c r="AF17" s="34"/>
+      <c r="Y17" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="Z17" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA17" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="AB17" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC17" s="7">
+        <f>(AA17+AA19)/2</f>
+        <v>2.75</v>
+      </c>
+      <c r="AD17" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE17" s="38">
+        <f>(AC17+AC21)/2</f>
+        <v>3.1749999999999998</v>
+      </c>
+      <c r="AF17" s="7" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="18" spans="1:32" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -2153,39 +2248,39 @@
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
       <c r="R18" s="9"/>
       <c r="S18" s="9"/>
       <c r="T18" s="9"/>
       <c r="U18" s="9"/>
       <c r="V18" s="9"/>
-      <c r="W18" s="37"/>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="34"/>
-      <c r="Z18" s="34"/>
-      <c r="AA18" s="34"/>
-      <c r="AB18" s="34"/>
-      <c r="AC18" s="34"/>
-      <c r="AD18" s="34"/>
-      <c r="AE18" s="34"/>
-      <c r="AF18" s="34"/>
+      <c r="W18" s="33"/>
+      <c r="X18" s="33"/>
+      <c r="Y18" s="32"/>
+      <c r="Z18" s="32"/>
+      <c r="AA18" s="32"/>
+      <c r="AB18" s="32"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="7"/>
+      <c r="AE18" s="38"/>
+      <c r="AF18" s="7"/>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="9" t="s">
         <v>45</v>
       </c>
       <c r="F19" s="9"/>
-      <c r="G19" s="25" t="s">
+      <c r="G19" s="10" t="s">
         <v>57</v>
       </c>
       <c r="H19" s="9"/>
-      <c r="I19" s="25" t="s">
+      <c r="I19" s="10" t="s">
         <v>50</v>
       </c>
       <c r="J19" s="9"/>
@@ -2201,15 +2296,15 @@
       <c r="N19" s="9">
         <v>2</v>
       </c>
-      <c r="O19" s="32">
+      <c r="O19" s="35">
         <f t="shared" ref="O19" si="6">L19*N19</f>
         <v>8</v>
       </c>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="32" t="s">
+      <c r="P19" s="35"/>
+      <c r="Q19" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="R19" s="25" t="s">
+      <c r="R19" s="10" t="s">
         <v>74</v>
       </c>
       <c r="S19" s="9"/>
@@ -2222,26 +2317,34 @@
       <c r="V19" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="W19" s="38">
+      <c r="W19" s="34">
         <v>2</v>
       </c>
-      <c r="X19" s="38" t="s">
+      <c r="X19" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="Y19" s="34"/>
-      <c r="Z19" s="34"/>
-      <c r="AA19" s="34"/>
-      <c r="AB19" s="34"/>
-      <c r="AC19" s="34"/>
-      <c r="AD19" s="34"/>
-      <c r="AE19" s="34"/>
-      <c r="AF19" s="34"/>
+      <c r="Y19" s="35">
+        <v>4</v>
+      </c>
+      <c r="Z19" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA19" s="35">
+        <v>4</v>
+      </c>
+      <c r="AB19" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC19" s="7"/>
+      <c r="AD19" s="7"/>
+      <c r="AE19" s="38"/>
+      <c r="AF19" s="7"/>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -2252,43 +2355,43 @@
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
       <c r="T20" s="9"/>
       <c r="U20" s="9"/>
       <c r="V20" s="9"/>
-      <c r="W20" s="38"/>
-      <c r="X20" s="38"/>
-      <c r="Y20" s="34"/>
-      <c r="Z20" s="34"/>
-      <c r="AA20" s="34"/>
-      <c r="AB20" s="34"/>
-      <c r="AC20" s="34"/>
-      <c r="AD20" s="34"/>
-      <c r="AE20" s="34"/>
-      <c r="AF20" s="34"/>
+      <c r="W20" s="34"/>
+      <c r="X20" s="34"/>
+      <c r="Y20" s="35"/>
+      <c r="Z20" s="35"/>
+      <c r="AA20" s="35"/>
+      <c r="AB20" s="35"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7"/>
+      <c r="AE20" s="38"/>
+      <c r="AF20" s="7"/>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="9"/>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="25"/>
+      <c r="D21" s="10"/>
       <c r="E21" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F21" s="9"/>
-      <c r="G21" s="25" t="s">
+      <c r="G21" s="10" t="s">
         <v>58</v>
       </c>
       <c r="H21" s="9"/>
-      <c r="I21" s="25" t="s">
+      <c r="I21" s="10" t="s">
         <v>24</v>
       </c>
       <c r="J21" s="9"/>
@@ -2304,15 +2407,15 @@
       <c r="N21" s="9">
         <v>4</v>
       </c>
-      <c r="O21" s="33">
+      <c r="O21" s="8">
         <f t="shared" ref="O21" si="7">L21*N21</f>
         <v>16</v>
       </c>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="33" t="s">
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="R21" s="25" t="s">
+      <c r="R21" s="10" t="s">
         <v>75</v>
       </c>
       <c r="S21" s="9"/>
@@ -2325,26 +2428,39 @@
       <c r="V21" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="W21" s="36">
+      <c r="W21" s="32">
         <v>5</v>
       </c>
-      <c r="X21" s="36" t="s">
+      <c r="X21" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="Y21" s="34"/>
-      <c r="Z21" s="34"/>
-      <c r="AA21" s="34"/>
-      <c r="AB21" s="34"/>
-      <c r="AC21" s="34"/>
-      <c r="AD21" s="34"/>
-      <c r="AE21" s="34"/>
-      <c r="AF21" s="34"/>
+      <c r="Y21" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="Z21" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA21" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="AB21" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC21" s="7">
+        <f>(AA21+AA23)/2</f>
+        <v>3.6</v>
+      </c>
+      <c r="AD21" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE21" s="38"/>
+      <c r="AF21" s="7"/>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -2355,39 +2471,39 @@
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
       <c r="R22" s="9"/>
       <c r="S22" s="9"/>
       <c r="T22" s="9"/>
       <c r="U22" s="9"/>
       <c r="V22" s="9"/>
-      <c r="W22" s="36"/>
-      <c r="X22" s="36"/>
-      <c r="Y22" s="34"/>
-      <c r="Z22" s="34"/>
-      <c r="AA22" s="34"/>
-      <c r="AB22" s="34"/>
-      <c r="AC22" s="34"/>
-      <c r="AD22" s="34"/>
-      <c r="AE22" s="34"/>
-      <c r="AF22" s="34"/>
+      <c r="W22" s="32"/>
+      <c r="X22" s="32"/>
+      <c r="Y22" s="7"/>
+      <c r="Z22" s="7"/>
+      <c r="AA22" s="7"/>
+      <c r="AB22" s="7"/>
+      <c r="AC22" s="7"/>
+      <c r="AD22" s="7"/>
+      <c r="AE22" s="38"/>
+      <c r="AF22" s="7"/>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
       <c r="E23" s="9" t="s">
         <v>27</v>
       </c>
       <c r="F23" s="9"/>
-      <c r="G23" s="25" t="s">
+      <c r="G23" s="10" t="s">
         <v>58</v>
       </c>
       <c r="H23" s="9"/>
-      <c r="I23" s="25" t="s">
+      <c r="I23" s="10" t="s">
         <v>51</v>
       </c>
       <c r="J23" s="9"/>
@@ -2403,15 +2519,15 @@
       <c r="N23" s="9">
         <v>4</v>
       </c>
-      <c r="O23" s="33">
+      <c r="O23" s="8">
         <f t="shared" ref="O23" si="8">L23*N23</f>
         <v>16</v>
       </c>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="33" t="s">
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="R23" s="25" t="s">
+      <c r="R23" s="10" t="s">
         <v>76</v>
       </c>
       <c r="S23" s="9"/>
@@ -2424,26 +2540,34 @@
       <c r="V23" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="W23" s="37">
+      <c r="W23" s="33">
         <v>4</v>
       </c>
-      <c r="X23" s="37" t="s">
+      <c r="X23" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="Y23" s="34"/>
-      <c r="Z23" s="34"/>
-      <c r="AA23" s="34"/>
-      <c r="AB23" s="34"/>
-      <c r="AC23" s="34"/>
-      <c r="AD23" s="34"/>
-      <c r="AE23" s="34"/>
-      <c r="AF23" s="34"/>
+      <c r="Y23" s="35">
+        <v>4</v>
+      </c>
+      <c r="Z23" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA23" s="35">
+        <v>4</v>
+      </c>
+      <c r="AB23" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC23" s="7"/>
+      <c r="AD23" s="7"/>
+      <c r="AE23" s="38"/>
+      <c r="AF23" s="7"/>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -2454,186 +2578,110 @@
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="33"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
       <c r="T24" s="9"/>
       <c r="U24" s="9"/>
       <c r="V24" s="9"/>
-      <c r="W24" s="37"/>
-      <c r="X24" s="37"/>
-      <c r="Y24" s="34"/>
-      <c r="Z24" s="34"/>
-      <c r="AA24" s="34"/>
-      <c r="AB24" s="34"/>
-      <c r="AC24" s="34"/>
-      <c r="AD24" s="34"/>
-      <c r="AE24" s="34"/>
-      <c r="AF24" s="34"/>
+      <c r="W24" s="33"/>
+      <c r="X24" s="33"/>
+      <c r="Y24" s="35"/>
+      <c r="Z24" s="35"/>
+      <c r="AA24" s="35"/>
+      <c r="AB24" s="35"/>
+      <c r="AC24" s="7"/>
+      <c r="AD24" s="7"/>
+      <c r="AE24" s="38"/>
+      <c r="AF24" s="7"/>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="258">
-    <mergeCell ref="AA21:AA22"/>
-    <mergeCell ref="AB21:AB22"/>
-    <mergeCell ref="AC21:AC22"/>
-    <mergeCell ref="AD21:AD22"/>
-    <mergeCell ref="AE21:AE22"/>
-    <mergeCell ref="AF21:AF22"/>
-    <mergeCell ref="AA23:AA24"/>
-    <mergeCell ref="AB23:AB24"/>
-    <mergeCell ref="AC23:AC24"/>
-    <mergeCell ref="AD23:AD24"/>
-    <mergeCell ref="AE23:AE24"/>
-    <mergeCell ref="AF23:AF24"/>
-    <mergeCell ref="AA17:AA18"/>
-    <mergeCell ref="AB17:AB18"/>
-    <mergeCell ref="AC17:AC18"/>
-    <mergeCell ref="AD17:AD18"/>
-    <mergeCell ref="AE17:AE18"/>
-    <mergeCell ref="AF17:AF18"/>
-    <mergeCell ref="AA19:AA20"/>
-    <mergeCell ref="AB19:AB20"/>
-    <mergeCell ref="AC19:AC20"/>
-    <mergeCell ref="AD19:AD20"/>
-    <mergeCell ref="AE19:AE20"/>
-    <mergeCell ref="AF19:AF20"/>
-    <mergeCell ref="AA13:AA14"/>
-    <mergeCell ref="AB13:AB14"/>
-    <mergeCell ref="AC13:AC14"/>
-    <mergeCell ref="AD13:AD14"/>
-    <mergeCell ref="AE13:AE14"/>
-    <mergeCell ref="AF13:AF14"/>
-    <mergeCell ref="AA15:AA16"/>
-    <mergeCell ref="AB15:AB16"/>
-    <mergeCell ref="AC15:AC16"/>
-    <mergeCell ref="AD15:AD16"/>
-    <mergeCell ref="AE15:AE16"/>
-    <mergeCell ref="AF15:AF16"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AA11:AA12"/>
-    <mergeCell ref="AB11:AB12"/>
-    <mergeCell ref="AC11:AC12"/>
-    <mergeCell ref="AD11:AD12"/>
-    <mergeCell ref="AE11:AE12"/>
-    <mergeCell ref="AF11:AF12"/>
-    <mergeCell ref="AA5:AA6"/>
-    <mergeCell ref="AB5:AB6"/>
-    <mergeCell ref="AC5:AC6"/>
-    <mergeCell ref="AD5:AD6"/>
-    <mergeCell ref="AE5:AE6"/>
-    <mergeCell ref="AF5:AF6"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="AD7:AD8"/>
-    <mergeCell ref="AE7:AE8"/>
-    <mergeCell ref="AF7:AF8"/>
-    <mergeCell ref="Y23:Y24"/>
-    <mergeCell ref="Z5:Z6"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="Z11:Z12"/>
-    <mergeCell ref="Z13:Z14"/>
-    <mergeCell ref="Z15:Z16"/>
-    <mergeCell ref="Z17:Z18"/>
-    <mergeCell ref="Z19:Z20"/>
-    <mergeCell ref="Z21:Z22"/>
-    <mergeCell ref="Z23:Z24"/>
-    <mergeCell ref="Y5:Y6"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Y11:Y12"/>
-    <mergeCell ref="Y13:Y14"/>
-    <mergeCell ref="Y15:Y16"/>
-    <mergeCell ref="Y17:Y18"/>
-    <mergeCell ref="Y19:Y20"/>
-    <mergeCell ref="Y21:Y22"/>
-    <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="Q17:Q18"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="Q21:Q22"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M23:M24"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="O5:P6"/>
-    <mergeCell ref="O7:P8"/>
-    <mergeCell ref="O9:P10"/>
-    <mergeCell ref="O11:P12"/>
-    <mergeCell ref="O13:P14"/>
-    <mergeCell ref="O15:P16"/>
-    <mergeCell ref="O17:P18"/>
-    <mergeCell ref="O19:P20"/>
-    <mergeCell ref="O21:P22"/>
-    <mergeCell ref="O23:P24"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="G17:H18"/>
-    <mergeCell ref="G19:H20"/>
-    <mergeCell ref="G21:H22"/>
-    <mergeCell ref="G23:H24"/>
-    <mergeCell ref="G7:H8"/>
-    <mergeCell ref="G9:H10"/>
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="E13:F14"/>
-    <mergeCell ref="E21:F22"/>
-    <mergeCell ref="E23:F24"/>
-    <mergeCell ref="E9:F10"/>
-    <mergeCell ref="E11:F12"/>
-    <mergeCell ref="E15:F16"/>
-    <mergeCell ref="E17:F18"/>
-    <mergeCell ref="E19:F20"/>
+  <mergeCells count="232">
+    <mergeCell ref="W21:W22"/>
+    <mergeCell ref="W23:W24"/>
+    <mergeCell ref="X5:X6"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="X15:X16"/>
+    <mergeCell ref="X17:X18"/>
+    <mergeCell ref="X19:X20"/>
+    <mergeCell ref="X21:X22"/>
+    <mergeCell ref="X23:X24"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="W7:W8"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="W11:W12"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="W15:W16"/>
+    <mergeCell ref="W17:W18"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="U23:U24"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="V11:V12"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="V15:V16"/>
+    <mergeCell ref="V17:V18"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="V21:V22"/>
+    <mergeCell ref="V23:V24"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="U15:U16"/>
+    <mergeCell ref="U17:U18"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="U21:U22"/>
+    <mergeCell ref="R23:S24"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="T17:T18"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="T21:T22"/>
+    <mergeCell ref="T23:T24"/>
+    <mergeCell ref="R5:S6"/>
+    <mergeCell ref="R7:S8"/>
+    <mergeCell ref="R9:S10"/>
+    <mergeCell ref="R11:S12"/>
+    <mergeCell ref="R13:S14"/>
+    <mergeCell ref="R15:S16"/>
+    <mergeCell ref="R17:S18"/>
+    <mergeCell ref="R19:S20"/>
+    <mergeCell ref="R21:S22"/>
+    <mergeCell ref="A2:B4"/>
+    <mergeCell ref="C2:D4"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="Y2:AF2"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="R2:X2"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="R3:S4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="G2:Q2"/>
+    <mergeCell ref="G3:H4"/>
+    <mergeCell ref="O3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="I3:J4"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="E2:F4"/>
     <mergeCell ref="A21:B24"/>
     <mergeCell ref="I5:J6"/>
     <mergeCell ref="A5:B16"/>
@@ -2656,86 +2704,136 @@
     <mergeCell ref="I9:J10"/>
     <mergeCell ref="I11:J12"/>
     <mergeCell ref="G15:H16"/>
-    <mergeCell ref="A2:B4"/>
-    <mergeCell ref="C2:D4"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="Y2:AF2"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="R2:X2"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="R3:S4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="G2:Q2"/>
-    <mergeCell ref="G3:H4"/>
-    <mergeCell ref="O3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="I3:J4"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="E2:F4"/>
-    <mergeCell ref="R23:S24"/>
-    <mergeCell ref="T5:T6"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="T11:T12"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="T17:T18"/>
-    <mergeCell ref="T19:T20"/>
-    <mergeCell ref="T21:T22"/>
-    <mergeCell ref="T23:T24"/>
-    <mergeCell ref="R5:S6"/>
-    <mergeCell ref="R7:S8"/>
-    <mergeCell ref="R9:S10"/>
-    <mergeCell ref="R11:S12"/>
-    <mergeCell ref="R13:S14"/>
-    <mergeCell ref="R15:S16"/>
-    <mergeCell ref="R17:S18"/>
-    <mergeCell ref="R19:S20"/>
-    <mergeCell ref="R21:S22"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="U11:U12"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="U15:U16"/>
-    <mergeCell ref="U17:U18"/>
-    <mergeCell ref="U19:U20"/>
-    <mergeCell ref="U21:U22"/>
-    <mergeCell ref="U23:U24"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="V11:V12"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="V15:V16"/>
-    <mergeCell ref="V17:V18"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="V21:V22"/>
-    <mergeCell ref="V23:V24"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="W5:W6"/>
-    <mergeCell ref="W7:W8"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="W11:W12"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="W15:W16"/>
-    <mergeCell ref="W17:W18"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:W22"/>
-    <mergeCell ref="W23:W24"/>
-    <mergeCell ref="X5:X6"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="X15:X16"/>
-    <mergeCell ref="X17:X18"/>
-    <mergeCell ref="X19:X20"/>
-    <mergeCell ref="X21:X22"/>
-    <mergeCell ref="X23:X24"/>
+    <mergeCell ref="G17:H18"/>
+    <mergeCell ref="G19:H20"/>
+    <mergeCell ref="G21:H22"/>
+    <mergeCell ref="G23:H24"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="G9:H10"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="E13:F14"/>
+    <mergeCell ref="E21:F22"/>
+    <mergeCell ref="E23:F24"/>
+    <mergeCell ref="E9:F10"/>
+    <mergeCell ref="E11:F12"/>
+    <mergeCell ref="E15:F16"/>
+    <mergeCell ref="E17:F18"/>
+    <mergeCell ref="E19:F20"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="O5:P6"/>
+    <mergeCell ref="O7:P8"/>
+    <mergeCell ref="O9:P10"/>
+    <mergeCell ref="O11:P12"/>
+    <mergeCell ref="O13:P14"/>
+    <mergeCell ref="O15:P16"/>
+    <mergeCell ref="O17:P18"/>
+    <mergeCell ref="O19:P20"/>
+    <mergeCell ref="O21:P22"/>
+    <mergeCell ref="O23:P24"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="Q17:Q18"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="Q21:Q22"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="Y23:Y24"/>
+    <mergeCell ref="Z5:Z6"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="Z11:Z12"/>
+    <mergeCell ref="Z13:Z14"/>
+    <mergeCell ref="Z15:Z16"/>
+    <mergeCell ref="Z17:Z18"/>
+    <mergeCell ref="Z19:Z20"/>
+    <mergeCell ref="Z21:Z22"/>
+    <mergeCell ref="Z23:Z24"/>
+    <mergeCell ref="Y5:Y6"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Y11:Y12"/>
+    <mergeCell ref="Y13:Y14"/>
+    <mergeCell ref="Y15:Y16"/>
+    <mergeCell ref="Y17:Y18"/>
+    <mergeCell ref="Y19:Y20"/>
+    <mergeCell ref="Y21:Y22"/>
+    <mergeCell ref="AA5:AA6"/>
+    <mergeCell ref="AB5:AB6"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="AC5:AC8"/>
+    <mergeCell ref="AD5:AD8"/>
+    <mergeCell ref="AE5:AE16"/>
+    <mergeCell ref="AF5:AF16"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AA11:AA12"/>
+    <mergeCell ref="AB11:AB12"/>
+    <mergeCell ref="AC9:AC12"/>
+    <mergeCell ref="AD9:AD12"/>
+    <mergeCell ref="AA13:AA14"/>
+    <mergeCell ref="AB13:AB14"/>
+    <mergeCell ref="AA15:AA16"/>
+    <mergeCell ref="AB15:AB16"/>
+    <mergeCell ref="AC13:AC16"/>
+    <mergeCell ref="AD13:AD16"/>
+    <mergeCell ref="AA17:AA18"/>
+    <mergeCell ref="AB17:AB18"/>
+    <mergeCell ref="AA19:AA20"/>
+    <mergeCell ref="AB19:AB20"/>
+    <mergeCell ref="AC17:AC20"/>
+    <mergeCell ref="AD17:AD20"/>
+    <mergeCell ref="AE17:AE24"/>
+    <mergeCell ref="AF17:AF24"/>
+    <mergeCell ref="AA21:AA22"/>
+    <mergeCell ref="AB21:AB22"/>
+    <mergeCell ref="AA23:AA24"/>
+    <mergeCell ref="AB23:AB24"/>
+    <mergeCell ref="AC21:AC24"/>
+    <mergeCell ref="AD21:AD24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>